<commit_message>
Refactoring formulas and template report
</commit_message>
<xml_diff>
--- a/Optic.Api/wwwroot/template/Formula.xlsx
+++ b/Optic.Api/wwwroot/template/Formula.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAB\OPTICA\ARQUITECTURA\ARQUITECTURA 1\optic\Optic.Api\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A237F8A-C46B-4C12-A4D4-B5EBF4077C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DE52ED-BBCA-4B4A-B5A0-365FD2F1BB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7856CE4B-3B11-43C1-AC86-06E476F1C136}"/>
   </bookViews>
@@ -153,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,87 +174,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF0070C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thick">
-        <color rgb="FF0070C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF0070C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color rgb="FF0070C0"/>
       </bottom>
       <diagonal/>
@@ -263,9 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -322,39 +242,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -754,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB634801-5C5D-41C3-B0E6-CCA3FC1E49A2}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,20 +758,20 @@
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
+      <c r="K9" s="17"/>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="20"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -887,10 +787,10 @@
       <c r="F11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="20"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="7"/>
       <c r="P11"/>
       <c r="Q11"/>
@@ -898,10 +798,10 @@
       <c r="S11"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
       <c r="L12" s="7"/>
       <c r="P12"/>
       <c r="Q12"/>
@@ -918,10 +818,10 @@
         <v>4</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="7"/>
       <c r="P13"/>
       <c r="Q13"/>
@@ -934,10 +834,10 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="19" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -956,6 +856,8 @@
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>

</xml_diff>